<commit_message>
Added untested slt/sltu code to ALU
</commit_message>
<xml_diff>
--- a/Project2b/TruthTable.xlsx
+++ b/Project2b/TruthTable.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="78">
   <si>
     <t>Instruction</t>
   </si>
@@ -255,6 +255,9 @@
   </si>
   <si>
     <t>J-Type</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -445,15 +448,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -471,6 +465,15 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -755,7 +758,7 @@
   <dimension ref="A1:U27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -812,7 +815,7 @@
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="19" t="s">
         <v>73</v>
       </c>
       <c r="B2" s="6" t="s">
@@ -862,7 +865,7 @@
       <c r="U2" s="1"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
+      <c r="A3" s="20"/>
       <c r="B3" s="6" t="s">
         <v>16</v>
       </c>
@@ -910,7 +913,7 @@
       <c r="U3" s="1"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
+      <c r="A4" s="20"/>
       <c r="B4" s="6" t="s">
         <v>22</v>
       </c>
@@ -958,7 +961,7 @@
       <c r="U4" s="1"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
+      <c r="A5" s="20"/>
       <c r="B5" s="6" t="s">
         <v>24</v>
       </c>
@@ -1006,7 +1009,7 @@
       <c r="U5" s="1"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
+      <c r="A6" s="20"/>
       <c r="B6" s="6" t="s">
         <v>17</v>
       </c>
@@ -1054,7 +1057,7 @@
       <c r="U6" s="1"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
+      <c r="A7" s="20"/>
       <c r="B7" s="6" t="s">
         <v>19</v>
       </c>
@@ -1102,7 +1105,7 @@
       <c r="U7" s="1"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
+      <c r="A8" s="20"/>
       <c r="B8" s="6" t="s">
         <v>23</v>
       </c>
@@ -1150,7 +1153,7 @@
       <c r="U8" s="1"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
+      <c r="A9" s="20"/>
       <c r="B9" s="6" t="s">
         <v>18</v>
       </c>
@@ -1198,7 +1201,7 @@
       <c r="U9" s="1"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
+      <c r="A10" s="20"/>
       <c r="B10" s="6" t="s">
         <v>20</v>
       </c>
@@ -1246,7 +1249,7 @@
       <c r="U10" s="1"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
+      <c r="A11" s="20"/>
       <c r="B11" s="6" t="s">
         <v>21</v>
       </c>
@@ -1294,7 +1297,7 @@
       <c r="U11" s="1"/>
     </row>
     <row r="12" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="15"/>
+      <c r="A12" s="21"/>
       <c r="B12" s="5" t="s">
         <v>13</v>
       </c>
@@ -1304,13 +1307,27 @@
       <c r="D12" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
+      <c r="E12" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="K12" s="10" t="s">
+        <v>77</v>
+      </c>
       <c r="L12" s="10"/>
       <c r="M12" s="10"/>
       <c r="N12" s="10"/>
@@ -1322,46 +1339,46 @@
       <c r="U12" s="1"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="19"/>
-      <c r="E13" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="F13" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="G13" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="H13" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="I13" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="J13" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="K13" s="18" t="s">
+      <c r="D13" s="16"/>
+      <c r="E13" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="H13" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="I13" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="J13" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="K13" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="L13" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="M13" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="N13" s="18"/>
-      <c r="O13" s="18"/>
-      <c r="P13" s="19" t="s">
+      <c r="L13" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="M13" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15"/>
+      <c r="P13" s="16" t="s">
         <v>63</v>
       </c>
       <c r="R13" s="1"/>
@@ -1370,7 +1387,7 @@
       <c r="U13" s="1"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
+      <c r="A14" s="20"/>
       <c r="B14" s="6" t="s">
         <v>26</v>
       </c>
@@ -1416,7 +1433,7 @@
       <c r="U14" s="1"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
+      <c r="A15" s="20"/>
       <c r="B15" s="6" t="s">
         <v>33</v>
       </c>
@@ -1462,7 +1479,7 @@
       <c r="U15" s="1"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
+      <c r="A16" s="20"/>
       <c r="B16" s="6" t="s">
         <v>34</v>
       </c>
@@ -1508,7 +1525,7 @@
       <c r="U16" s="1"/>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
+      <c r="A17" s="20"/>
       <c r="B17" s="6" t="s">
         <v>27</v>
       </c>
@@ -1554,7 +1571,7 @@
       <c r="U17" s="1"/>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
+      <c r="A18" s="20"/>
       <c r="B18" s="6" t="s">
         <v>32</v>
       </c>
@@ -1600,7 +1617,7 @@
       <c r="U18" s="1"/>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
+      <c r="A19" s="20"/>
       <c r="B19" s="6" t="s">
         <v>36</v>
       </c>
@@ -1646,7 +1663,7 @@
       <c r="U19" s="1"/>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
+      <c r="A20" s="20"/>
       <c r="B20" s="6" t="s">
         <v>31</v>
       </c>
@@ -1692,7 +1709,7 @@
       <c r="U20" s="1"/>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
+      <c r="A21" s="20"/>
       <c r="B21" s="6" t="s">
         <v>28</v>
       </c>
@@ -1732,7 +1749,7 @@
       <c r="U21" s="1"/>
     </row>
     <row r="22" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="15"/>
+      <c r="A22" s="21"/>
       <c r="B22" s="5" t="s">
         <v>29</v>
       </c>
@@ -1772,46 +1789,46 @@
       <c r="U22" s="1"/>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C23" s="18" t="s">
+      <c r="C23" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="D23" s="19"/>
-      <c r="E23" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="F23" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="G23" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="H23" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="I23" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="J23" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="K23" s="18" t="s">
+      <c r="D23" s="16"/>
+      <c r="E23" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="G23" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="H23" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="I23" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="J23" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="K23" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="L23" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="M23" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="N23" s="18"/>
-      <c r="O23" s="18"/>
-      <c r="P23" s="19" t="s">
+      <c r="L23" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="M23" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="N23" s="15"/>
+      <c r="O23" s="15"/>
+      <c r="P23" s="16" t="s">
         <v>63</v>
       </c>
       <c r="R23" s="1"/>
@@ -1820,7 +1837,7 @@
       <c r="U23" s="1"/>
     </row>
     <row r="24" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="15"/>
+      <c r="A24" s="21"/>
       <c r="B24" s="5" t="s">
         <v>35</v>
       </c>
@@ -1866,30 +1883,30 @@
       <c r="U24" s="1"/>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A25" s="13" t="s">
+      <c r="A25" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="B25" s="17" t="s">
+      <c r="B25" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C25" s="18" t="s">
+      <c r="C25" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="D25" s="19"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
-      <c r="H25" s="18"/>
-      <c r="I25" s="18"/>
-      <c r="J25" s="18"/>
-      <c r="K25" s="18"/>
-      <c r="L25" s="18"/>
-      <c r="M25" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="N25" s="18"/>
-      <c r="O25" s="18"/>
-      <c r="P25" s="19" t="s">
+      <c r="D25" s="16"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
+      <c r="I25" s="15"/>
+      <c r="J25" s="15"/>
+      <c r="K25" s="15"/>
+      <c r="L25" s="15"/>
+      <c r="M25" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="N25" s="15"/>
+      <c r="O25" s="15"/>
+      <c r="P25" s="16" t="s">
         <v>63</v>
       </c>
       <c r="R25" s="1"/>
@@ -1898,7 +1915,7 @@
       <c r="U25" s="1"/>
     </row>
     <row r="26" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="15"/>
+      <c r="A26" s="21"/>
       <c r="B26" s="5" t="s">
         <v>12</v>
       </c>
@@ -1926,50 +1943,50 @@
       <c r="U26" s="1"/>
     </row>
     <row r="27" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="16" t="s">
+      <c r="A27" s="13" t="s">
         <v>14</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C27" s="20" t="s">
+      <c r="C27" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="D27" s="21"/>
-      <c r="E27" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="F27" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="G27" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="H27" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="I27" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="J27" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="K27" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="L27" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="M27" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="N27" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="O27" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="P27" s="21" t="s">
+      <c r="D27" s="18"/>
+      <c r="E27" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="F27" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="G27" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="H27" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="I27" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="J27" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="K27" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="L27" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="M27" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="N27" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="O27" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="P27" s="18" t="s">
         <v>62</v>
       </c>
     </row>

</xml_diff>